<commit_message>
Final Import Form HR and running Power BI
</commit_message>
<xml_diff>
--- a/template Excel/HR/Application.xlsx
+++ b/template Excel/HR/Application.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ToolControlDatabase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ToolControlDatabase\template Excel\HR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1CA41E-F02A-4EA7-8D59-197805D63D1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6CB9509-05AF-4419-9334-3C3F5F7D6E87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{B0E9E192-1C31-4093-A38F-8DE1BBD0FF18}"/>
   </bookViews>
@@ -38,39 +38,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="55">
   <si>
-    <t xml:space="preserve"> FullName</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> DateOfBirth</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Gender</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Address</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Level</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> PhoneNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Email</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ApplicationDate</t>
-  </si>
-  <si>
     <t>PassCv</t>
   </si>
   <si>
-    <t xml:space="preserve"> RecruitmentChannelId</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> JobPositionId </t>
-  </si>
-  <si>
     <t>InterviewDate</t>
   </si>
   <si>
@@ -80,9 +50,6 @@
     <t>HireDate</t>
   </si>
   <si>
-    <t xml:space="preserve">ApplicantId </t>
-  </si>
-  <si>
     <t>ApplicationId</t>
   </si>
   <si>
@@ -201,6 +168,39 @@
   </si>
   <si>
     <t>bui.k@example.com</t>
+  </si>
+  <si>
+    <t>ApplicantId</t>
+  </si>
+  <si>
+    <t>FullName</t>
+  </si>
+  <si>
+    <t>DateOfBirth</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>PhoneNumber</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>RecruitmentChannelId</t>
+  </si>
+  <si>
+    <t>JobPositionId</t>
+  </si>
+  <si>
+    <t>ApplicationDate</t>
   </si>
 </sst>
 </file>
@@ -581,7 +581,7 @@
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,52 +606,52 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="C1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="N1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="O1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="P1" t="s">
         <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -662,25 +662,25 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="D2" s="2">
         <v>32918</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="G2" s="1">
         <v>987654321</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="J2" s="1">
         <v>1</v>
@@ -692,13 +692,13 @@
         <v>45296</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="N2" s="2">
         <v>45301</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="P2" s="2">
         <v>45323</v>
@@ -712,25 +712,25 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="D3" s="2">
         <v>33746</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="G3" s="1">
         <v>912345678</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="J3" s="1">
         <v>2</v>
@@ -742,13 +742,13 @@
         <v>45334</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="N3" s="2">
         <v>45340</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="P3" s="2">
         <v>45352</v>
@@ -762,25 +762,25 @@
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="D4" s="2">
         <v>32450</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="G4" s="1">
         <v>901234567</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="J4" s="1">
         <v>3</v>
@@ -792,13 +792,13 @@
         <v>45376</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="N4" s="2">
         <v>45381</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="P4" s="2">
         <v>45352</v>
@@ -812,25 +812,25 @@
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="D5" s="2">
         <v>34897</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="G5" s="1">
         <v>981122334</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="J5" s="1">
         <v>4</v>
@@ -842,13 +842,13 @@
         <v>45384</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="N5" s="2">
         <v>45390</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="P5" s="2">
         <v>45413</v>
@@ -862,25 +862,25 @@
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="D6" s="2">
         <v>33491</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="G6" s="1">
         <v>976543210</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="J6" s="1">
         <v>1</v>
@@ -892,13 +892,13 @@
         <v>45428</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="N6" s="2">
         <v>45433</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="P6" s="2">
         <v>45444</v>
@@ -912,25 +912,25 @@
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="D7" s="2">
         <v>32132</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="G7" s="1">
         <v>965432109</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="J7" s="1">
         <v>2</v>
@@ -942,13 +942,13 @@
         <v>45461</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="N7" s="2">
         <v>45468</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="P7" s="2">
         <v>45352</v>
@@ -962,25 +962,25 @@
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="D8" s="2">
         <v>34429</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="G8" s="1">
         <v>954321098</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="J8" s="1">
         <v>3</v>
@@ -992,13 +992,13 @@
         <v>45484</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="N8" s="2">
         <v>45488</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="P8" s="2">
         <v>45505</v>
@@ -1012,25 +1012,25 @@
         <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="D9" s="2">
         <v>33114</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="G9" s="1">
         <v>943210987</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="J9" s="1">
         <v>4</v>
@@ -1042,13 +1042,13 @@
         <v>45507</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="N9" s="2">
         <v>45514</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="P9" s="2">
         <v>45536</v>
@@ -1062,25 +1062,25 @@
         <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="D10" s="2">
         <v>34047</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="G10" s="1">
         <v>932109876</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="J10" s="1">
         <v>1</v>
@@ -1092,13 +1092,13 @@
         <v>45542</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="N10" s="2">
         <v>45550</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="P10" s="2">
         <v>45352</v>
@@ -1112,25 +1112,25 @@
         <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="D11" s="2">
         <v>35246</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="G11" s="1">
         <v>921098765</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="J11" s="1">
         <v>2</v>
@@ -1142,13 +1142,13 @@
         <v>45587</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="N11" s="2">
         <v>45592</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="P11" s="2">
         <v>45611</v>

</xml_diff>